<commit_message>
close #50 and #52
</commit_message>
<xml_diff>
--- a/src/tests/option-car-ev-phv-re.test-cases.xlsx
+++ b/src/tests/option-car-ev-phv-re.test-cases.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/JibungotoPlanet-backend/src/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC7E004-02A8-524B-821F-0BC4514A4DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA170D4-27A9-354E-B904-50E476E6DB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="2" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
   <sheets>
     <sheet name="answers" sheetId="24" r:id="rId1"/>
     <sheet name="car-ev-phv-re01" sheetId="2" r:id="rId2"/>
+    <sheet name="car-ev-phv-re02" sheetId="25" r:id="rId3"/>
+    <sheet name="car-ev-phv-re03" sheetId="26" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="135">
   <si>
     <t>case</t>
     <phoneticPr fontId="1"/>
@@ -658,6 +660,200 @@
       <t>ヘイキン</t>
     </rPh>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ev</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>housingAnswer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>electricityIntensityKey</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>30-renewable</t>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>phv</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>car-ev-phv-re02</t>
+  </si>
+  <si>
+    <t>car-ev-phv-re02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>car-ev-phv-re03</t>
+  </si>
+  <si>
+    <t>car-ev-phv-re03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>質問票で算出した「車種による自動車運転のGHG排出原単位（再エネ充電考慮）」</t>
+    <rPh sb="0" eb="3">
+      <t>シツモンヒョウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>サンシュツ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ジュウデン</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>コウリョ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>kgCO2e/km-passenger</t>
+  </si>
+  <si>
+    <t>↓</t>
+  </si>
+  <si>
+    <t>電動化後＋１００％再エネ充電後の自動車運転のGHG排出原単位(EVとPHVの平均）</t>
+    <rPh sb="0" eb="2">
+      <t>デンドウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ジュウデン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="16" eb="21">
+      <t>ジドウシャウンテン</t>
+    </rPh>
+    <rPh sb="25" eb="30">
+      <t>ハイシュツゲンタンイ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ヘイキン</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>↑自家用車、カーシェアリングの運転時の原単位を上記の比率で削減</t>
+    <rPh sb="1" eb="5">
+      <t>ジカヨウシャ</t>
+    </rPh>
+    <rPh sb="15" eb="18">
+      <t>ウンテンジ</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>ゲンタンイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ジョウキ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヒリツ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>サクゲン</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>質問票で算出した「車種による自動車製造時のGHG排出原単位」</t>
+    <rPh sb="0" eb="3">
+      <t>シツモンヒョウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>サンシュツ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>セイゾウ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ジ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>kgCO2e/台</t>
+    <rPh sb="7" eb="8">
+      <t>ダイ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>電動化後の自動車製造時のGHG排出原単位(EVとPHVの平均）</t>
+    <rPh sb="0" eb="2">
+      <t>デンドウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>ジドウシャ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>セイゾウ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="15" eb="20">
+      <t>ハイシュツゲンタンイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ヘイキン</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>↑自家用車、カーシェアリングの購入時の原単位を上記の比率で削減</t>
+    <rPh sb="1" eb="5">
+      <t>ジカヨウシャ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>コウニュウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>ゲンタンイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ジョウキ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヒリツ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>サクゲン</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
   </si>
 </sst>
 </file>
@@ -770,7 +966,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -792,6 +988,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1066,7 +1268,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1146,6 +1348,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="桁区切り" xfId="1" builtinId="6"/>
@@ -1162,934 +1367,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>139701</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5892800" cy="564257"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="テキスト ボックス 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A36A99F-EF9B-9E45-A08B-FC9FD05BD254}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8737601" y="127000"/>
-          <a:ext cx="5892800" cy="564257"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>  最初のケースで</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>PUSH</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>した後、同じデータに対して</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>PUT</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>していくため、一度</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>housingAnswer</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>を設定するとその後も引き継がれる。そのため、最初に</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>housingAnswer</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>なしを検証。</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="13472150" cy="4275914"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="テキスト ボックス 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AB319C8-B53B-2E42-8EC9-BBD6EFAA2DFD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8813800" y="635000"/>
-          <a:ext cx="13472150" cy="4275914"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>hasPrivateCar: Boolean # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>自家用車を持っている場合は</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>true</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>carIntensityFactorKey: String # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>自家用車の種類</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>; gasoline_driving-factor|light_driving-factor|hv_driving-factor|phv_driving-factor|ev_driving-factor|unknown_driving-factor</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>carChargingKey: String # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>自宅充電の割合</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>; charge-almost-at-home|use-charging-spots-occasionally|use-charging-spots-sometimes|use-charging-spots-usually|unknown</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>carPassengersKey: String # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>平均乗車人数</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>; 1_private-car-factor|1-2_private-car-factor|2_private-car-factor|2-3_private-car-factor|3_private-car-factor|3-4_private-car-factor|4-more_private-car-factor|unknown_private-car-factor</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>privateCarAnnualMileage: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>年間の走行距離 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>km/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>年</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>trainWeeklyTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>鉄道の移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>週</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>busWeeklyTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>バスの移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>週</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>motorbikeWeeklyTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>バイクの移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>週</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>otherCarWeeklyTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>タクシー、レンタカー、カーシェアの移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>週</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>hasWeeklyTravelingTime: Boolean # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>自家用車以外の普通の移動手段をスキップした場合は</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>false</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>mileageByAreaFirstKey: String # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>住んでいる地域の規模 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>city-50k-150k|major-city-or-metropolitan-area|city-150k-more|area-less-than-50k|unknown</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>otherCarAnnualTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>タクシー、レンタカー、カーシェアの移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>年</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>trainAnnualTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>鉄道の移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>年</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>busAnnualTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>バスの移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>年</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>motorbikeAnnualTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>バイクの移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>年</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>airplaneAnnualTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>飛行機の移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>年</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>ferryAnnualTravelingTime: Float # </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>フェリーの移動時間 時間</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>年</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2392,15 +1669,15 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
@@ -2697,7 +1974,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>52</v>
@@ -2710,12 +1987,623 @@
       </c>
       <c r="E18" s="2" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="1">
+        <v>20</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="1">
+        <v>20</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="1">
+        <v>20</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="1">
+        <v>20</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="1">
+        <v>5</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="1">
+        <v>20</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="1">
+        <v>20</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="1">
+        <v>20</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="1">
+        <v>20</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="1">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="E54" s="49" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2726,7 +2614,7 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -3515,4 +3403,1600 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3C41B0-D9F2-104F-A62F-7986CCC280EA}">
+  <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="47"/>
+      <c r="N1" s="48"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="30">
+        <v>0.1240646347585653</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="35"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="37"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="31">
+        <v>3.132655726355852E-2</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="31">
+        <v>8.2993045321770986E-2</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.4246913320994587</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="M5" s="43">
+        <v>7.1304478209538585E-2</v>
+      </c>
+      <c r="N5" s="44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="21" thickBot="1">
+      <c r="A6" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0.23623051809728152</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="24"/>
+      <c r="M6" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="32">
+        <v>1.4255463957350388E-2</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="M7" s="38">
+        <v>2.5653594403779831E-2</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="21" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1.4282910430915969E-2</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="31">
+        <v>5.7043135066020045E-2</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="31">
+        <v>1.3134541259492592E-2</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="M10" s="38">
+        <v>9200</v>
+      </c>
+      <c r="N10" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="21" thickBot="1">
+      <c r="A11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="31">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" ht="21" thickBot="1">
+      <c r="A12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="41">
+        <v>9878.351775398678</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="M12" s="45">
+        <v>8027.5</v>
+      </c>
+      <c r="N12" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="21" thickBot="1">
+      <c r="A13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="31">
+        <v>979.65757829210111</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="25"/>
+      <c r="M13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N13" s="20"/>
+    </row>
+    <row r="14" spans="1:14" ht="21" thickBot="1">
+      <c r="A14" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="41">
+        <v>16.807142130209751</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" s="25"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="31">
+        <v>1.6480883122109475</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" s="25"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="20"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="31">
+        <v>1.9658018365725201</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L16" s="25"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="20"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="34">
+        <v>2.3243850285273413</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" s="26"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="D2:D11 D13 D15:D17">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CB5D165D-EAC2-DA47-AC6A-E149BD3C6916}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5002A350-3EEE-5344-85A0-343652AE9510}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AA8E22D4-15A8-114B-A3A3-3DC3B15ABB8C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CB5D165D-EAC2-DA47-AC6A-E149BD3C6916}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D2:D11 D13 D15:D17</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5002A350-3EEE-5344-85A0-343652AE9510}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AA8E22D4-15A8-114B-A3A3-3DC3B15ABB8C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D14</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378605B9-C063-6744-B8EE-959A80A18BE9}">
+  <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="47"/>
+      <c r="N1" s="48"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="30">
+        <v>0.1240646347585653</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="35"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="37"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="31">
+        <v>3.132655726355852E-2</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="31">
+        <v>8.2993045321770986E-2</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.4246913320994587</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="M5" s="43">
+        <v>8.0244008352885532E-2</v>
+      </c>
+      <c r="N5" s="44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="21" thickBot="1">
+      <c r="A6" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0.42951003290414824</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="24"/>
+      <c r="M6" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="32">
+        <v>3.2646100665687912E-2</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="M7" s="38">
+        <v>2.5653594403779831E-2</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="21" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="33">
+        <v>3.2708955185303742E-2</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="31">
+        <v>5.7043135066020045E-2</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="31">
+        <v>1.3134541259492592E-2</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="M10" s="38">
+        <v>9200</v>
+      </c>
+      <c r="N10" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="21" thickBot="1">
+      <c r="A11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="31">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" ht="21" thickBot="1">
+      <c r="A12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="41">
+        <v>9878.351775398678</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="M12" s="45">
+        <v>8027.5</v>
+      </c>
+      <c r="N12" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="21" thickBot="1">
+      <c r="A13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="31">
+        <v>979.65757829210111</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="25"/>
+      <c r="M13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N13" s="20"/>
+    </row>
+    <row r="14" spans="1:14" ht="21" thickBot="1">
+      <c r="A14" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="41">
+        <v>16.807142130209751</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" s="25"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="31">
+        <v>1.6480883122109475</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" s="25"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="20"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="31">
+        <v>1.9658018365725201</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L16" s="25"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="20"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="34">
+        <v>2.3243850285273413</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" s="26"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="D2:D11 D13 D15:D17">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1E68B43D-2689-3949-9F0E-C2B58507114D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{81AEA08F-7C7F-5647-8BC3-71EB3949770F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0179813D-54C6-9E4B-88A0-2A312B68D80C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1E68B43D-2689-3949-9F0E-C2B58507114D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D2:D11 D13 D15:D17</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{81AEA08F-7C7F-5647-8BC3-71EB3949770F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0179813D-54C6-9E4B-88A0-2A312B68D80C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D14</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>